<commit_message>
Added visuals for Madrid Region and LEZ analysis in 00-OD-Prep.
</commit_message>
<xml_diff>
--- a/data-raw/Environmental label.xlsx
+++ b/data-raw/Environmental label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcmasteru365-my.sharepoint.com/personal/soukhoa_mcmaster_ca/Documents/05. PhD Research/05_Madrid-ZBE-LEZ/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1997A052-BF77-450D-BCF5-B204EB4755DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{1997A052-BF77-450D-BCF5-B204EB4755DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{20DC0F60-30BD-4BCF-AED8-7E84A3684368}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10B3CFAA-3080-47E6-A27B-72815110960E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{10B3CFAA-3080-47E6-A27B-72815110960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -249,20 +247,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -278,7 +276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -576,15 +574,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33906CEE-74CE-43FF-AAD6-08C02BE536DC}">
   <dimension ref="B1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101:B107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="11.5546875" style="4"/>
-    <col min="8" max="8" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="3"/>
+    <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -597,13 +595,13 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -620,13 +618,13 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.9</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0.16015441423296406</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.17111757928567106</v>
       </c>
     </row>
@@ -641,13 +639,13 @@
       <c r="F4">
         <v>290</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.72459639126305797</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>-1.5249194503977992E-2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>-4.2860294512709896E-3</v>
       </c>
     </row>
@@ -662,13 +660,13 @@
       <c r="F5">
         <v>326</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.70709793351302785</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>-3.2747652254008108E-2</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>-2.1784487201301106E-2</v>
       </c>
     </row>
@@ -683,13 +681,13 @@
       <c r="F6">
         <v>219</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.76677316293929709</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>2.692757717226113E-2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>3.7890742224968132E-2</v>
       </c>
     </row>
@@ -704,13 +702,13 @@
       <c r="F7">
         <v>254</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>0.75786463298379414</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>1.8019047216758177E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>2.898221226946518E-2</v>
       </c>
     </row>
@@ -725,13 +723,13 @@
       <c r="F8">
         <v>318</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.71908127208480566</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>-2.0764313682230306E-2</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>-9.8011486295233041E-3</v>
       </c>
     </row>
@@ -746,18 +744,18 @@
       <c r="F9">
         <v>142</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.78549848942598188</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>4.565290365894592E-2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>5.6616068711652923E-2</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
@@ -769,18 +767,18 @@
       <c r="F10">
         <v>49</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.83389830508474572</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>6.348658142808139E-2</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>0.10501588437041676</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>1</v>
       </c>
@@ -790,18 +788,18 @@
       <c r="F11">
         <v>201</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0.77054794520547942</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1.362215488150964E-4</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>4.1665524491150463E-2</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
+      <c r="B12" s="7"/>
       <c r="C12" t="s">
         <v>2</v>
       </c>
@@ -811,18 +809,18 @@
       <c r="F12">
         <v>249</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.75659824046920821</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>-1.3813483187456121E-2</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>2.7715819754879245E-2</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>3</v>
       </c>
@@ -832,18 +830,18 @@
       <c r="F13">
         <v>173</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.75804195804195806</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>-1.2369765614706263E-2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>2.9159537327629104E-2</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>4</v>
       </c>
@@ -853,18 +851,18 @@
       <c r="F14">
         <v>171</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>0.79618593563766393</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>2.5774211980999606E-2</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>6.7303514923334973E-2</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
+      <c r="B15" s="7"/>
       <c r="C15" t="s">
         <v>5</v>
       </c>
@@ -874,18 +872,18 @@
       <c r="F15">
         <v>204</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.76578645235361653</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>-4.6252713030477954E-3</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>3.6904031639287571E-2</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>6</v>
       </c>
@@ -895,18 +893,18 @@
       <c r="F16">
         <v>237</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>0.74211099020674642</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>-2.8300733449917903E-2</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>1.3228569492417463E-2</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -916,18 +914,18 @@
       <c r="F17">
         <v>32</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>0.83505154639175261</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>6.4639822735088281E-2</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>0.10616912567742365</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
@@ -939,18 +937,18 @@
       <c r="F18">
         <v>8</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>0.86885245901639341</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>0.10840146161830144</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>0.13997003830206445</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>1</v>
       </c>
@@ -960,18 +958,18 @@
       <c r="F19">
         <v>297</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>0.73243243243243239</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>-2.8018564965659576E-2</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>3.5500117181034296E-3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>2</v>
       </c>
@@ -981,18 +979,18 @@
       <c r="F20">
         <v>206</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>0.75990675990675993</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>-5.4423749133203358E-4</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>3.1024339192430972E-2</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
+      <c r="B21" s="7"/>
       <c r="C21" t="s">
         <v>3</v>
       </c>
@@ -1002,18 +1000,18 @@
       <c r="F21">
         <v>223</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>0.76746611053180391</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>7.0151131337119477E-3</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>3.8583689817474953E-2</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
+      <c r="B22" s="7"/>
       <c r="C22" t="s">
         <v>4</v>
       </c>
@@ -1023,18 +1021,18 @@
       <c r="F22">
         <v>241</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>0.764187866927593</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>3.7368695295010301E-3</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>3.5305446213264036E-2</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
+      <c r="B23" s="7"/>
       <c r="C23" t="s">
         <v>5</v>
       </c>
@@ -1044,18 +1042,18 @@
       <c r="F23">
         <v>169</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>0.8</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>3.9549002601908079E-2</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>7.1117579285671084E-2</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
+      <c r="B24" s="7"/>
       <c r="C24" t="s">
         <v>6</v>
       </c>
@@ -1065,18 +1063,18 @@
       <c r="F24">
         <v>237</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>0.7395604395604396</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>-2.0890557837652368E-2</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <v>1.0678018846110637E-2</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
@@ -1088,18 +1086,18 @@
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>0.95454545454545459</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <v>0.2111253084795871</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="3">
         <v>0.22566303383112563</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
+      <c r="B26" s="7"/>
       <c r="C26" t="s">
         <v>1</v>
       </c>
@@ -1109,18 +1107,18 @@
       <c r="F26">
         <v>340</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>0.7473997028231798</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <v>3.9795567573123192E-3</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
         <v>1.8517282108850841E-2</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
+      <c r="B27" s="7"/>
       <c r="C27" t="s">
         <v>2</v>
       </c>
@@ -1130,18 +1128,18 @@
       <c r="F27">
         <v>317</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>0.74578989574979948</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>2.3697496839319987E-3</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="3">
         <v>1.6907475035470521E-2</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
+      <c r="B28" s="7"/>
       <c r="C28" t="s">
         <v>3</v>
       </c>
@@ -1151,18 +1149,18 @@
       <c r="F28">
         <v>220</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>0.75582685904550495</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <v>1.2406712979637469E-2</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
         <v>2.6944438331175991E-2</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
+      <c r="B29" s="7"/>
       <c r="C29" t="s">
         <v>4</v>
       </c>
@@ -1172,18 +1170,18 @@
       <c r="F29">
         <v>374</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>0.71921921921921927</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <v>-2.4200926846648207E-2</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="3">
         <v>-9.6632014951096856E-3</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
+      <c r="B30" s="7"/>
       <c r="C30" t="s">
         <v>5</v>
       </c>
@@ -1193,18 +1191,18 @@
       <c r="F30">
         <v>246</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>0.76770538243626063</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>2.4285236370393148E-2</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="3">
         <v>3.882296172193167E-2</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
+      <c r="B31" s="7"/>
       <c r="C31" t="s">
         <v>6</v>
       </c>
@@ -1214,18 +1212,18 @@
       <c r="F31">
         <v>364</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>0.73037037037037034</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <v>-1.3049775695497146E-2</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="3">
         <v>1.4879496560413763E-3</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C32" t="s">
@@ -1237,18 +1235,18 @@
       <c r="F32">
         <v>1</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>0.9</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <v>0.16734402286077155</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <v>0.17111757928567106</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
+      <c r="B33" s="7"/>
       <c r="C33" t="s">
         <v>1</v>
       </c>
@@ -1258,18 +1256,18 @@
       <c r="F33">
         <v>300</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>0.72924187725631773</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <v>-3.4140998829107483E-3</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <v>3.5945654198876742E-4</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
+      <c r="B34" s="7"/>
       <c r="C34" t="s">
         <v>2</v>
       </c>
@@ -1279,18 +1277,18 @@
       <c r="F34">
         <v>313</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>0.7254385964912281</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <v>-7.217380648000371E-3</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="3">
         <v>-3.4438242231008553E-3</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
+      <c r="B35" s="7"/>
       <c r="C35" t="s">
         <v>3</v>
       </c>
@@ -1300,18 +1298,18 @@
       <c r="F35">
         <v>233</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>0.75186368477103305</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <v>1.9207707631804571E-2</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="3">
         <v>2.2981264056704087E-2</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
+      <c r="B36" s="7"/>
       <c r="C36" t="s">
         <v>4</v>
       </c>
@@ -1321,18 +1319,18 @@
       <c r="F36">
         <v>322</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>0.71654929577464788</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <v>-1.61066813645806E-2</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <v>-1.2333124939681084E-2</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
+      <c r="B37" s="7"/>
       <c r="C37" t="s">
         <v>5</v>
       </c>
@@ -1342,18 +1340,18 @@
       <c r="F37">
         <v>344</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>0.7121338912133891</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <v>-2.0522085925839373E-2</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <v>-1.6748529500939857E-2</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
+      <c r="B38" s="7"/>
       <c r="C38" t="s">
         <v>6</v>
       </c>
@@ -1363,18 +1361,18 @@
       <c r="F38">
         <v>171</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>0.77821011673151752</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <v>4.5554139592289045E-2</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <v>4.932769601718856E-2</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
@@ -1386,18 +1384,18 @@
       <c r="F39">
         <v>8</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>0.89189189189189189</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <v>0.1443006740748014</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <v>0.16300947117756293</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
+      <c r="B40" s="7"/>
       <c r="C40" t="s">
         <v>1</v>
       </c>
@@ -1407,18 +1405,18 @@
       <c r="F40">
         <v>216</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>0.76774193548387093</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <v>2.0150717666780449E-2</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="3">
         <v>3.885951476954197E-2</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
+      <c r="B41" s="7"/>
       <c r="C41" t="s">
         <v>2</v>
       </c>
@@ -1428,18 +1426,18 @@
       <c r="F41">
         <v>369</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <v>0.73848334514528702</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <v>-9.107872671803463E-3</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="3">
         <v>9.6009244309580577E-3</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
+      <c r="B42" s="7"/>
       <c r="C42" t="s">
         <v>3</v>
       </c>
@@ -1449,18 +1447,18 @@
       <c r="F42">
         <v>299</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>0.75867635189669091</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="3">
         <v>1.1085134079600434E-2</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="3">
         <v>2.9793931182361955E-2</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="3"/>
+      <c r="B43" s="7"/>
       <c r="C43" t="s">
         <v>4</v>
       </c>
@@ -1470,18 +1468,18 @@
       <c r="F43">
         <v>247</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>0.73034934497816595</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <v>-1.7241872838924532E-2</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="3">
         <v>1.4669242638369884E-3</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
+      <c r="B44" s="7"/>
       <c r="C44" t="s">
         <v>5</v>
       </c>
@@ -1491,18 +1489,18 @@
       <c r="F44">
         <v>236</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <v>0.73363431151241532</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <v>-1.3956906304675165E-2</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="3">
         <v>4.7518907980863556E-3</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="3"/>
+      <c r="B45" s="7"/>
       <c r="C45" t="s">
         <v>6</v>
       </c>
@@ -1512,18 +1510,18 @@
       <c r="F45">
         <v>223</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="3">
         <v>0.74514285714285711</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="3">
         <v>-2.4483606742333741E-3</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45" s="3">
         <v>1.6260436428528147E-2</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C46" t="s">
@@ -1535,18 +1533,18 @@
       <c r="F46">
         <v>9</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="3">
         <v>0.83636363636363631</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="3">
         <v>9.3442954376979581E-2</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46" s="3">
         <v>0.10748121564930735</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="3"/>
+      <c r="B47" s="7"/>
       <c r="C47" t="s">
         <v>1</v>
       </c>
@@ -1556,18 +1554,18 @@
       <c r="F47">
         <v>255</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="3">
         <v>0.73792394655704008</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="3">
         <v>-4.99673542961665E-3</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47" s="3">
         <v>9.0415258427111178E-3</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
+      <c r="B48" s="7"/>
       <c r="C48" t="s">
         <v>2</v>
       </c>
@@ -1577,18 +1575,18 @@
       <c r="F48">
         <v>262</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="3">
         <v>0.75650557620817849</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48" s="3">
         <v>1.3584894221521759E-2</v>
       </c>
-      <c r="I48" s="4">
+      <c r="I48" s="3">
         <v>2.7623155493849527E-2</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="3"/>
+      <c r="B49" s="7"/>
       <c r="C49" t="s">
         <v>3</v>
       </c>
@@ -1598,18 +1596,18 @@
       <c r="F49">
         <v>273</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="3">
         <v>0.74722222222222223</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="3">
         <v>4.3015402355655041E-3</v>
       </c>
-      <c r="I49" s="4">
+      <c r="I49" s="3">
         <v>1.8339801507893272E-2</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="3"/>
+      <c r="B50" s="7"/>
       <c r="C50" t="s">
         <v>4</v>
       </c>
@@ -1619,18 +1617,18 @@
       <c r="F50">
         <v>342</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="3">
         <v>0.7432432432432432</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50" s="3">
         <v>3.2256125658647328E-4</v>
       </c>
-      <c r="I50" s="4">
+      <c r="I50" s="3">
         <v>1.4360822528914241E-2</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
+      <c r="B51" s="7"/>
       <c r="C51" t="s">
         <v>5</v>
       </c>
@@ -1640,18 +1638,18 @@
       <c r="F51">
         <v>326</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="3">
         <v>0.7206512425021423</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51" s="3">
         <v>-2.2269439484514431E-2</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I51" s="3">
         <v>-8.2311782121866628E-3</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="3"/>
+      <c r="B52" s="7"/>
       <c r="C52" t="s">
         <v>6</v>
       </c>
@@ -1661,18 +1659,18 @@
       <c r="F52">
         <v>267</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="3">
         <v>0.74858757062146897</v>
       </c>
-      <c r="H52" s="4">
+      <c r="H52" s="3">
         <v>5.6668886348122394E-3</v>
       </c>
-      <c r="I52" s="4">
+      <c r="I52" s="3">
         <v>1.9705149907140007E-2</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C53" t="s">
@@ -1684,18 +1682,18 @@
       <c r="F53">
         <v>70</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="3">
         <v>0.80056980056980054</v>
       </c>
-      <c r="H53" s="4">
+      <c r="H53" s="3">
         <v>6.3390313390313313E-2</v>
       </c>
-      <c r="I53" s="4">
+      <c r="I53" s="3">
         <v>7.1687379855471578E-2</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="3"/>
+      <c r="B54" s="7"/>
       <c r="C54" t="s">
         <v>1</v>
       </c>
@@ -1705,18 +1703,18 @@
       <c r="F54">
         <v>103</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="3">
         <v>0.72606382978723405</v>
       </c>
-      <c r="H54" s="4">
+      <c r="H54" s="3">
         <v>-1.1115657392253175E-2</v>
       </c>
-      <c r="I54" s="4">
+      <c r="I54" s="3">
         <v>-2.8185909270949105E-3</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="3"/>
+      <c r="B55" s="7"/>
       <c r="C55" t="s">
         <v>2</v>
       </c>
@@ -1726,18 +1724,18 @@
       <c r="F55">
         <v>79</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="3">
         <v>0.81922196796338675</v>
       </c>
-      <c r="H55" s="4">
+      <c r="H55" s="3">
         <v>8.204248078389953E-2</v>
       </c>
-      <c r="I55" s="4">
+      <c r="I55" s="3">
         <v>9.0339547249057794E-2</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="3"/>
+      <c r="B56" s="7"/>
       <c r="C56" t="s">
         <v>3</v>
       </c>
@@ -1747,18 +1745,18 @@
       <c r="F56">
         <v>338</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="3">
         <v>0.72249589490968802</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H56" s="3">
         <v>-1.4683592269799206E-2</v>
       </c>
-      <c r="I56" s="4">
+      <c r="I56" s="3">
         <v>-6.3865258046409412E-3</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B57" s="3"/>
+      <c r="B57" s="7"/>
       <c r="C57" t="s">
         <v>4</v>
       </c>
@@ -1768,18 +1766,18 @@
       <c r="F57">
         <v>293</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="3">
         <v>0.7222748815165877</v>
       </c>
-      <c r="H57" s="4">
+      <c r="H57" s="3">
         <v>-1.4904605662899528E-2</v>
       </c>
-      <c r="I57" s="4">
+      <c r="I57" s="3">
         <v>-6.6075391977412634E-3</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B58" s="3"/>
+      <c r="B58" s="7"/>
       <c r="C58" t="s">
         <v>5</v>
       </c>
@@ -1789,18 +1787,18 @@
       <c r="F58">
         <v>290</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="3">
         <v>0.73048327137546465</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H58" s="3">
         <v>-6.6962158040225761E-3</v>
       </c>
-      <c r="I58" s="4">
+      <c r="I58" s="3">
         <v>1.6008506611356887E-3</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B59" s="3"/>
+      <c r="B59" s="7"/>
       <c r="C59" t="s">
         <v>6</v>
       </c>
@@ -1810,18 +1808,18 @@
       <c r="F59">
         <v>413</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="3">
         <v>0.7161512027491409</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="3">
         <v>-2.1028284430346322E-2</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I59" s="3">
         <v>-1.2731217965188057E-2</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
+      <c r="B60" s="7"/>
       <c r="C60" t="s">
         <v>8</v>
       </c>
@@ -1831,18 +1829,18 @@
       <c r="F60">
         <v>346</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="3">
         <v>0.71847030105777054</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="3">
         <v>-1.8709186121716681E-2</v>
       </c>
-      <c r="I60" s="4">
+      <c r="I60" s="3">
         <v>-1.0412119656558416E-2</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B61" s="3"/>
+      <c r="B61" s="7"/>
       <c r="C61" t="s">
         <v>9</v>
       </c>
@@ -1852,18 +1850,18 @@
       <c r="F61">
         <v>159</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="3">
         <v>0.79051383399209485</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="3">
         <v>5.3334346812607625E-2</v>
       </c>
-      <c r="I61" s="4">
+      <c r="I61" s="3">
         <v>6.163141327776589E-2</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C62" t="s">
@@ -1875,18 +1873,18 @@
       <c r="F62">
         <v>5</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="3">
         <v>0.9</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="3">
         <v>0.1252280105116711</v>
       </c>
-      <c r="I62" s="4">
+      <c r="I62" s="3">
         <v>0.17111757928567106</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B63" s="3"/>
+      <c r="B63" s="7"/>
       <c r="C63" t="s">
         <v>1</v>
       </c>
@@ -1896,18 +1894,18 @@
       <c r="F63">
         <v>173</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="3">
         <v>0.76398362892223737</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="3">
         <v>-1.0788360566091559E-2</v>
       </c>
-      <c r="I63" s="4">
+      <c r="I63" s="3">
         <v>3.5101208207908408E-2</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
+      <c r="B64" s="7"/>
       <c r="C64" t="s">
         <v>2</v>
       </c>
@@ -1917,18 +1915,18 @@
       <c r="F64">
         <v>321</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="3">
         <v>0.73047858942065491</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H64" s="3">
         <v>-4.4293400067674016E-2</v>
       </c>
-      <c r="I64" s="4">
+      <c r="I64" s="3">
         <v>1.5961687063259511E-3</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B65" s="3"/>
+      <c r="B65" s="7"/>
       <c r="C65" t="s">
         <v>3</v>
       </c>
@@ -1938,18 +1936,18 @@
       <c r="F65">
         <v>243</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="3">
         <v>0.76338851022395326</v>
       </c>
-      <c r="H65" s="4">
+      <c r="H65" s="3">
         <v>-1.1383479264375662E-2</v>
       </c>
-      <c r="I65" s="4">
+      <c r="I65" s="3">
         <v>3.4506089509624305E-2</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B66" s="3"/>
+      <c r="B66" s="7"/>
       <c r="C66" t="s">
         <v>4</v>
       </c>
@@ -1959,18 +1957,18 @@
       <c r="F66">
         <v>221</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="3">
         <v>0.76287553648068673</v>
       </c>
-      <c r="H66" s="4">
+      <c r="H66" s="3">
         <v>-1.1896453007642194E-2</v>
       </c>
-      <c r="I66" s="4">
+      <c r="I66" s="3">
         <v>3.3993115766357773E-2</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B67" s="3"/>
+      <c r="B67" s="7"/>
       <c r="C67" t="s">
         <v>5</v>
       </c>
@@ -1980,18 +1978,18 @@
       <c r="F67">
         <v>110</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="3">
         <v>0.85155195681511475</v>
       </c>
-      <c r="H67" s="4">
+      <c r="H67" s="3">
         <v>7.6779967326785825E-2</v>
       </c>
-      <c r="I67" s="4">
+      <c r="I67" s="3">
         <v>0.12266953610078579</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B68" s="3"/>
+      <c r="B68" s="7"/>
       <c r="C68" t="s">
         <v>6</v>
       </c>
@@ -2001,18 +1999,18 @@
       <c r="F68">
         <v>74</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="3">
         <v>0.8671454219030521</v>
       </c>
-      <c r="H68" s="4">
+      <c r="H68" s="3">
         <v>9.2373432414723178E-2</v>
       </c>
-      <c r="I68" s="4">
+      <c r="I68" s="3">
         <v>0.13826300118872314</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B69" s="3"/>
+      <c r="B69" s="7"/>
       <c r="C69" t="s">
         <v>8</v>
       </c>
@@ -2022,18 +2020,18 @@
       <c r="F69">
         <v>310</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="3">
         <v>0.74959612277867527</v>
       </c>
-      <c r="H69" s="4">
+      <c r="H69" s="3">
         <v>-2.517586670965366E-2</v>
       </c>
-      <c r="I69" s="4">
+      <c r="I69" s="3">
         <v>2.0713702064346307E-2</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C70" t="s">
@@ -2045,18 +2043,18 @@
       <c r="F70">
         <v>8</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="3">
         <v>0.87692307692307692</v>
       </c>
-      <c r="H70" s="4">
+      <c r="H70" s="3">
         <v>0.15490627020038783</v>
       </c>
-      <c r="I70" s="4">
+      <c r="I70" s="3">
         <v>0.14804065620874796</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B71" s="3"/>
+      <c r="B71" s="7"/>
       <c r="C71" t="s">
         <v>1</v>
       </c>
@@ -2066,18 +2064,18 @@
       <c r="F71">
         <v>188</v>
       </c>
-      <c r="G71" s="4">
+      <c r="G71" s="3">
         <v>0.73333333333333328</v>
       </c>
-      <c r="H71" s="4">
+      <c r="H71" s="3">
         <v>1.1316526610644195E-2</v>
       </c>
-      <c r="I71" s="4">
+      <c r="I71" s="3">
         <v>4.4509126190043213E-3</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B72" s="3"/>
+      <c r="B72" s="7"/>
       <c r="C72" t="s">
         <v>2</v>
       </c>
@@ -2087,18 +2085,18 @@
       <c r="F72">
         <v>285</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="3">
         <v>0.715852442671984</v>
       </c>
-      <c r="H72" s="4">
+      <c r="H72" s="3">
         <v>-6.1643640507050845E-3</v>
       </c>
-      <c r="I72" s="4">
+      <c r="I72" s="3">
         <v>-1.3029978042344958E-2</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B73" s="3"/>
+      <c r="B73" s="7"/>
       <c r="C73" t="s">
         <v>3</v>
       </c>
@@ -2108,18 +2106,18 @@
       <c r="F73">
         <v>257</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="3">
         <v>0.7254273504273504</v>
       </c>
-      <c r="H73" s="4">
+      <c r="H73" s="3">
         <v>3.4105437046613174E-3</v>
       </c>
-      <c r="I73" s="4">
+      <c r="I73" s="3">
         <v>-3.4550702869785566E-3</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B74" s="3"/>
+      <c r="B74" s="7"/>
       <c r="C74" t="s">
         <v>4</v>
       </c>
@@ -2129,18 +2127,18 @@
       <c r="F74">
         <v>334</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="3">
         <v>0.69828364950316169</v>
       </c>
-      <c r="H74" s="4">
+      <c r="H74" s="3">
         <v>-2.3733157219527401E-2</v>
       </c>
-      <c r="I74" s="4">
+      <c r="I74" s="3">
         <v>-3.0598771211167275E-2</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B75" s="3"/>
+      <c r="B75" s="7"/>
       <c r="C75" t="s">
         <v>5</v>
       </c>
@@ -2150,18 +2148,18 @@
       <c r="F75">
         <v>172</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="3">
         <v>0.74018126888217528</v>
       </c>
-      <c r="H75" s="4">
+      <c r="H75" s="3">
         <v>1.8164462159486194E-2</v>
       </c>
-      <c r="I75" s="4">
+      <c r="I75" s="3">
         <v>1.129884816784632E-2</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B76" s="3"/>
+      <c r="B76" s="7"/>
       <c r="C76" t="s">
         <v>6</v>
       </c>
@@ -2171,18 +2169,18 @@
       <c r="F76">
         <v>78</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="3">
         <v>0.81603773584905659</v>
       </c>
-      <c r="H76" s="4">
+      <c r="H76" s="3">
         <v>9.4020929126367503E-2</v>
       </c>
-      <c r="I76" s="4">
+      <c r="I76" s="3">
         <v>8.7155315134727629E-2</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B77" s="3"/>
+      <c r="B77" s="7"/>
       <c r="C77" t="s">
         <v>8</v>
       </c>
@@ -2192,18 +2190,18 @@
       <c r="F77">
         <v>332</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G77" s="3">
         <v>0.68320610687022898</v>
       </c>
-      <c r="H77" s="4">
+      <c r="H77" s="3">
         <v>-3.8810699852460107E-2</v>
       </c>
-      <c r="I77" s="4">
+      <c r="I77" s="3">
         <v>-4.5676313844099981E-2</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C78" t="s">
@@ -2215,18 +2213,18 @@
       <c r="F78">
         <v>29</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="3">
         <v>0.83888888888888891</v>
       </c>
-      <c r="H78" s="4">
+      <c r="H78" s="3">
         <v>0.11181561113548832</v>
       </c>
-      <c r="I78" s="4">
+      <c r="I78" s="3">
         <v>0.11000646817455995</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B79" s="3"/>
+      <c r="B79" s="7"/>
       <c r="C79" t="s">
         <v>1</v>
       </c>
@@ -2236,18 +2234,18 @@
       <c r="F79">
         <v>229</v>
       </c>
-      <c r="G79" s="4">
+      <c r="G79" s="3">
         <v>0.73122065727699526</v>
       </c>
-      <c r="H79" s="4">
+      <c r="H79" s="3">
         <v>4.1473795235946742E-3</v>
       </c>
-      <c r="I79" s="4">
+      <c r="I79" s="3">
         <v>2.338236562666296E-3</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B80" s="3"/>
+      <c r="B80" s="7"/>
       <c r="C80" t="s">
         <v>2</v>
       </c>
@@ -2257,18 +2255,18 @@
       <c r="F80">
         <v>238</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G80" s="3">
         <v>0.73555555555555552</v>
       </c>
-      <c r="H80" s="4">
+      <c r="H80" s="3">
         <v>8.4822778021549361E-3</v>
       </c>
-      <c r="I80" s="4">
+      <c r="I80" s="3">
         <v>6.6731348412265579E-3</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B81" s="3"/>
+      <c r="B81" s="7"/>
       <c r="C81" t="s">
         <v>3</v>
       </c>
@@ -2278,18 +2276,18 @@
       <c r="F81">
         <v>298</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G81" s="3">
         <v>0.708984375</v>
       </c>
-      <c r="H81" s="4">
+      <c r="H81" s="3">
         <v>-1.8088902753400582E-2</v>
       </c>
-      <c r="I81" s="4">
+      <c r="I81" s="3">
         <v>-1.989804571432896E-2</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B82" s="3"/>
+      <c r="B82" s="7"/>
       <c r="C82" t="s">
         <v>4</v>
       </c>
@@ -2299,18 +2297,18 @@
       <c r="F82">
         <v>273</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G82" s="3">
         <v>0.72256097560975607</v>
       </c>
-      <c r="H82" s="4">
+      <c r="H82" s="3">
         <v>-4.5123021436445088E-3</v>
       </c>
-      <c r="I82" s="4">
+      <c r="I82" s="3">
         <v>-6.321445104572887E-3</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B83" s="3"/>
+      <c r="B83" s="7"/>
       <c r="C83" t="s">
         <v>5</v>
       </c>
@@ -2320,18 +2318,18 @@
       <c r="F83">
         <v>248</v>
       </c>
-      <c r="G83" s="4">
+      <c r="G83" s="3">
         <v>0.7185017026106697</v>
       </c>
-      <c r="H83" s="4">
+      <c r="H83" s="3">
         <v>-8.5715751427308806E-3</v>
       </c>
-      <c r="I83" s="4">
+      <c r="I83" s="3">
         <v>-1.0380718103659259E-2</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B84" s="3"/>
+      <c r="B84" s="7"/>
       <c r="C84" t="s">
         <v>6</v>
       </c>
@@ -2341,18 +2339,18 @@
       <c r="F84">
         <v>322</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G84" s="3">
         <v>0.72121212121212119</v>
       </c>
-      <c r="H84" s="4">
+      <c r="H84" s="3">
         <v>-5.8611565412793887E-3</v>
       </c>
-      <c r="I84" s="4">
+      <c r="I84" s="3">
         <v>-7.6702995022077669E-3</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B85" s="3"/>
+      <c r="B85" s="7"/>
       <c r="C85" t="s">
         <v>8</v>
       </c>
@@ -2362,18 +2360,18 @@
       <c r="F85">
         <v>229</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G85" s="3">
         <v>0.73403019744483156</v>
       </c>
-      <c r="H85" s="4">
+      <c r="H85" s="3">
         <v>6.9569196914309739E-3</v>
       </c>
-      <c r="I85" s="4">
+      <c r="I85" s="3">
         <v>5.1477767305025957E-3</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C86" t="s">
@@ -2385,18 +2383,18 @@
       <c r="F86">
         <v>10</v>
       </c>
-      <c r="G86" s="4">
+      <c r="G86" s="3">
         <v>0.81481481481481477</v>
       </c>
-      <c r="H86" s="4">
+      <c r="H86" s="3">
         <v>8.6055341340542713E-2</v>
       </c>
-      <c r="I86" s="4">
+      <c r="I86" s="3">
         <v>8.5932394100485809E-2</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B87" s="3"/>
+      <c r="B87" s="7"/>
       <c r="C87" t="s">
         <v>1</v>
       </c>
@@ -2406,18 +2404,18 @@
       <c r="F87">
         <v>233</v>
       </c>
-      <c r="G87" s="4">
+      <c r="G87" s="3">
         <v>0.70506329113924049</v>
       </c>
-      <c r="H87" s="4">
+      <c r="H87" s="3">
         <v>-2.3696182335031568E-2</v>
       </c>
-      <c r="I87" s="4">
+      <c r="I87" s="3">
         <v>-2.3819129575088471E-2</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B88" s="3"/>
+      <c r="B88" s="7"/>
       <c r="C88" t="s">
         <v>2</v>
       </c>
@@ -2427,18 +2425,18 @@
       <c r="F88">
         <v>176</v>
       </c>
-      <c r="G88" s="4">
+      <c r="G88" s="3">
         <v>0.71335504885993484</v>
       </c>
-      <c r="H88" s="4">
+      <c r="H88" s="3">
         <v>-1.540442461433722E-2</v>
       </c>
-      <c r="I88" s="4">
+      <c r="I88" s="3">
         <v>-1.5527371854394123E-2</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B89" s="3"/>
+      <c r="B89" s="7"/>
       <c r="C89" t="s">
         <v>3</v>
       </c>
@@ -2448,18 +2446,18 @@
       <c r="F89">
         <v>225</v>
       </c>
-      <c r="G89" s="4">
+      <c r="G89" s="3">
         <v>0.72153465346534651</v>
       </c>
-      <c r="H89" s="4">
+      <c r="H89" s="3">
         <v>-7.2248200089255477E-3</v>
       </c>
-      <c r="I89" s="4">
+      <c r="I89" s="3">
         <v>-7.3477672489824508E-3</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B90" s="3"/>
+      <c r="B90" s="7"/>
       <c r="C90" t="s">
         <v>4</v>
       </c>
@@ -2469,18 +2467,18 @@
       <c r="F90">
         <v>176</v>
       </c>
-      <c r="G90" s="4">
+      <c r="G90" s="3">
         <v>0.74566473988439308</v>
       </c>
-      <c r="H90" s="4">
+      <c r="H90" s="3">
         <v>1.6905266410121023E-2</v>
       </c>
-      <c r="I90" s="4">
+      <c r="I90" s="3">
         <v>1.6782319170064119E-2</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B91" s="3"/>
+      <c r="B91" s="7"/>
       <c r="C91" t="s">
         <v>5</v>
       </c>
@@ -2490,18 +2488,18 @@
       <c r="F91">
         <v>214</v>
       </c>
-      <c r="G91" s="4">
+      <c r="G91" s="3">
         <v>0.72669220945083013</v>
       </c>
-      <c r="H91" s="4">
+      <c r="H91" s="3">
         <v>-2.0672640234419282E-3</v>
       </c>
-      <c r="I91" s="4">
+      <c r="I91" s="3">
         <v>-2.1902112634988313E-3</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B92" s="3"/>
+      <c r="B92" s="7"/>
       <c r="C92" t="s">
         <v>6</v>
       </c>
@@ -2511,18 +2509,18 @@
       <c r="F92">
         <v>158</v>
       </c>
-      <c r="G92" s="4">
+      <c r="G92" s="3">
         <v>0.74267100977198697</v>
       </c>
-      <c r="H92" s="4">
+      <c r="H92" s="3">
         <v>1.391153629771491E-2</v>
       </c>
-      <c r="I92" s="4">
+      <c r="I92" s="3">
         <v>1.3788589057658007E-2</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B93" s="3"/>
+      <c r="B93" s="7"/>
       <c r="C93" t="s">
         <v>8</v>
       </c>
@@ -2532,18 +2530,18 @@
       <c r="F93">
         <v>168</v>
       </c>
-      <c r="G93" s="4">
+      <c r="G93" s="3">
         <v>0.74506828528072833</v>
       </c>
-      <c r="H93" s="4">
+      <c r="H93" s="3">
         <v>1.6308811806456269E-2</v>
       </c>
-      <c r="I93" s="4">
+      <c r="I93" s="3">
         <v>1.6185864566399366E-2</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C94" t="s">
@@ -2555,18 +2553,18 @@
       <c r="F94">
         <v>52</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="3">
         <v>0.77192982456140347</v>
       </c>
-      <c r="H94" s="4">
+      <c r="H94" s="3">
         <v>6.4188644156788821E-2</v>
       </c>
-      <c r="I94" s="4">
+      <c r="I94" s="3">
         <v>4.3047403847074506E-2</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B95" s="3"/>
+      <c r="B95" s="7"/>
       <c r="C95" t="s">
         <v>1</v>
       </c>
@@ -2576,18 +2574,18 @@
       <c r="F95">
         <v>292</v>
       </c>
-      <c r="G95" s="4">
+      <c r="G95" s="3">
         <v>0.68803418803418803</v>
       </c>
-      <c r="H95" s="4">
+      <c r="H95" s="3">
         <v>-1.9706992370426613E-2</v>
       </c>
-      <c r="I95" s="4">
+      <c r="I95" s="3">
         <v>-4.0848232680140928E-2</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B96" s="3"/>
+      <c r="B96" s="7"/>
       <c r="C96" t="s">
         <v>2</v>
       </c>
@@ -2597,18 +2595,18 @@
       <c r="F96">
         <v>265</v>
       </c>
-      <c r="G96" s="4">
+      <c r="G96" s="3">
         <v>0.71413160733549086</v>
       </c>
-      <c r="H96" s="4">
+      <c r="H96" s="3">
         <v>6.3904269308762141E-3</v>
       </c>
-      <c r="I96" s="4">
+      <c r="I96" s="3">
         <v>-1.4750813378838101E-2</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B97" s="3"/>
+      <c r="B97" s="7"/>
       <c r="C97" t="s">
         <v>3</v>
       </c>
@@ -2618,18 +2616,18 @@
       <c r="F97">
         <v>285</v>
       </c>
-      <c r="G97" s="4">
+      <c r="G97" s="3">
         <v>0.70769230769230773</v>
       </c>
-      <c r="H97" s="4">
+      <c r="H97" s="3">
         <v>-4.8872712306913257E-5</v>
       </c>
-      <c r="I97" s="4">
+      <c r="I97" s="3">
         <v>-2.1190113022021229E-2</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B98" s="3"/>
+      <c r="B98" s="7"/>
       <c r="C98" t="s">
         <v>4</v>
       </c>
@@ -2639,18 +2637,18 @@
       <c r="F98">
         <v>309</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G98" s="3">
         <v>0.70173745173745172</v>
       </c>
-      <c r="H98" s="4">
+      <c r="H98" s="3">
         <v>-6.003728667162922E-3</v>
       </c>
-      <c r="I98" s="4">
+      <c r="I98" s="3">
         <v>-2.7144968976877237E-2</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B99" s="3"/>
+      <c r="B99" s="7"/>
       <c r="C99" t="s">
         <v>5</v>
       </c>
@@ -2660,18 +2658,18 @@
       <c r="F99">
         <v>235</v>
       </c>
-      <c r="G99" s="4">
+      <c r="G99" s="3">
         <v>0.71990464839094159</v>
       </c>
-      <c r="H99" s="4">
+      <c r="H99" s="3">
         <v>1.2163467986326948E-2</v>
       </c>
-      <c r="I99" s="4">
+      <c r="I99" s="3">
         <v>-8.9777723233873674E-3</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B100" s="3"/>
+      <c r="B100" s="7"/>
       <c r="C100" t="s">
         <v>6</v>
       </c>
@@ -2681,18 +2679,18 @@
       <c r="F100">
         <v>310</v>
       </c>
-      <c r="G100" s="4">
+      <c r="G100" s="3">
         <v>0.70192307692307687</v>
       </c>
-      <c r="H100" s="4">
+      <c r="H100" s="3">
         <v>-5.818103481537773E-3</v>
       </c>
-      <c r="I100" s="4">
+      <c r="I100" s="3">
         <v>-2.6959343791252088E-2</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C101" t="s">
@@ -2704,18 +2702,18 @@
       <c r="F101">
         <v>27</v>
       </c>
-      <c r="G101" s="4">
+      <c r="G101" s="3">
         <v>0.8392857142857143</v>
       </c>
-      <c r="H101" s="4">
+      <c r="H101" s="3">
         <v>7.3371956585508991E-2</v>
       </c>
-      <c r="I101" s="4">
+      <c r="I101" s="3">
         <v>0.11040329357138534</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B102" s="3"/>
+      <c r="B102" s="7"/>
       <c r="C102" t="s">
         <v>1</v>
       </c>
@@ -2725,18 +2723,18 @@
       <c r="F102">
         <v>118</v>
       </c>
-      <c r="G102" s="4">
+      <c r="G102" s="3">
         <v>0.78467153284671531</v>
       </c>
-      <c r="H102" s="4">
+      <c r="H102" s="3">
         <v>1.8757775146510003E-2</v>
       </c>
-      <c r="I102" s="4">
+      <c r="I102" s="3">
         <v>5.5789112132386354E-2</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B103" s="3"/>
+      <c r="B103" s="7"/>
       <c r="C103" t="s">
         <v>2</v>
       </c>
@@ -2746,18 +2744,18 @@
       <c r="F103">
         <v>68</v>
       </c>
-      <c r="G103" s="4">
+      <c r="G103" s="3">
         <v>0.81914893617021278</v>
       </c>
-      <c r="H103" s="4">
+      <c r="H103" s="3">
         <v>5.3235178470007471E-2</v>
       </c>
-      <c r="I103" s="4">
+      <c r="I103" s="3">
         <v>9.0266515455883822E-2</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B104" s="3"/>
+      <c r="B104" s="7"/>
       <c r="C104" t="s">
         <v>3</v>
       </c>
@@ -2767,18 +2765,18 @@
       <c r="F104">
         <v>212</v>
       </c>
-      <c r="G104" s="4">
+      <c r="G104" s="3">
         <v>0.74881516587677721</v>
       </c>
-      <c r="H104" s="4">
+      <c r="H104" s="3">
         <v>-1.70985918234281E-2</v>
       </c>
-      <c r="I104" s="4">
+      <c r="I104" s="3">
         <v>1.9932745162448251E-2</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B105" s="3"/>
+      <c r="B105" s="7"/>
       <c r="C105" t="s">
         <v>4</v>
       </c>
@@ -2788,18 +2786,18 @@
       <c r="F105">
         <v>174</v>
       </c>
-      <c r="G105" s="4">
+      <c r="G105" s="3">
         <v>0.76098901098901095</v>
       </c>
-      <c r="H105" s="4">
+      <c r="H105" s="3">
         <v>-4.924746711194361E-3</v>
       </c>
-      <c r="I105" s="4">
+      <c r="I105" s="3">
         <v>3.210659027468199E-2</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B106" s="3"/>
+      <c r="B106" s="7"/>
       <c r="C106" t="s">
         <v>5</v>
       </c>
@@ -2809,18 +2807,18 @@
       <c r="F106">
         <v>166</v>
       </c>
-      <c r="G106" s="4">
+      <c r="G106" s="3">
         <v>0.74223602484472051</v>
       </c>
-      <c r="H106" s="4">
+      <c r="H106" s="3">
         <v>-2.3677732855484801E-2</v>
       </c>
-      <c r="I106" s="4">
+      <c r="I106" s="3">
         <v>1.335360413039155E-2</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B107" s="3"/>
+      <c r="B107" s="7"/>
       <c r="C107" t="s">
         <v>6</v>
       </c>
@@ -2830,18 +2828,18 @@
       <c r="F107">
         <v>147</v>
       </c>
-      <c r="G107" s="4">
+      <c r="G107" s="3">
         <v>0.75</v>
       </c>
-      <c r="H107" s="4">
+      <c r="H107" s="3">
         <v>-1.5913757700205311E-2</v>
       </c>
-      <c r="I107" s="4">
+      <c r="I107" s="3">
         <v>2.111757928567104E-2</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C108" t="s">
@@ -2853,18 +2851,18 @@
       <c r="F108">
         <v>36</v>
       </c>
-      <c r="G108" s="4">
+      <c r="G108" s="3">
         <v>0.79428571428571426</v>
       </c>
-      <c r="H108" s="4">
+      <c r="H108" s="3">
         <v>4.8100566778084608E-2</v>
       </c>
-      <c r="I108" s="4">
+      <c r="I108" s="3">
         <v>6.5403293571385301E-2</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B109" s="3"/>
+      <c r="B109" s="7"/>
       <c r="C109" t="s">
         <v>1</v>
       </c>
@@ -2874,18 +2872,18 @@
       <c r="F109">
         <v>309</v>
       </c>
-      <c r="G109" s="4">
+      <c r="G109" s="3">
         <v>0.70655270655270652</v>
       </c>
-      <c r="H109" s="4">
+      <c r="H109" s="3">
         <v>-3.9632440954923132E-2</v>
       </c>
-      <c r="I109" s="4">
+      <c r="I109" s="3">
         <v>-2.2329714161622438E-2</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B110" s="3"/>
+      <c r="B110" s="7"/>
       <c r="C110" t="s">
         <v>2</v>
       </c>
@@ -2895,18 +2893,18 @@
       <c r="F110">
         <v>373</v>
       </c>
-      <c r="G110" s="4">
+      <c r="G110" s="3">
         <v>0.69699431356620634</v>
       </c>
-      <c r="H110" s="4">
+      <c r="H110" s="3">
         <v>-4.9190833941423318E-2</v>
       </c>
-      <c r="I110" s="4">
+      <c r="I110" s="3">
         <v>-3.1888107148122624E-2</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B111" s="3"/>
+      <c r="B111" s="7"/>
       <c r="C111" t="s">
         <v>3</v>
       </c>
@@ -2916,18 +2914,18 @@
       <c r="F111">
         <v>224</v>
       </c>
-      <c r="G111" s="4">
+      <c r="G111" s="3">
         <v>0.73553719008264462</v>
       </c>
-      <c r="H111" s="4">
+      <c r="H111" s="3">
         <v>-1.0647957424985033E-2</v>
       </c>
-      <c r="I111" s="4">
+      <c r="I111" s="3">
         <v>6.6547693683156606E-3</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B112" s="3"/>
+      <c r="B112" s="7"/>
       <c r="C112" t="s">
         <v>4</v>
       </c>
@@ -2937,18 +2935,18 @@
       <c r="F112">
         <v>235</v>
       </c>
-      <c r="G112" s="4">
+      <c r="G112" s="3">
         <v>0.7280092592592593</v>
       </c>
-      <c r="H112" s="4">
+      <c r="H112" s="3">
         <v>-1.8175888248370353E-2</v>
       </c>
-      <c r="I112" s="4">
+      <c r="I112" s="3">
         <v>-8.7316145506965981E-4</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B113" s="3"/>
+      <c r="B113" s="7"/>
       <c r="C113" t="s">
         <v>5</v>
       </c>
@@ -2958,18 +2956,18 @@
       <c r="F113">
         <v>212</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="3">
         <v>0.7633928571428571</v>
       </c>
-      <c r="H113" s="4">
+      <c r="H113" s="3">
         <v>1.7207709635227442E-2</v>
       </c>
-      <c r="I113" s="4">
+      <c r="I113" s="3">
         <v>3.4510436428528135E-2</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B114" s="3"/>
+      <c r="B114" s="7"/>
       <c r="C114" t="s">
         <v>6</v>
       </c>
@@ -2979,18 +2977,18 @@
       <c r="F114">
         <v>214</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G114" s="3">
         <v>0.76035834266517355</v>
       </c>
-      <c r="H114" s="4">
+      <c r="H114" s="3">
         <v>1.4173195157543894E-2</v>
       </c>
-      <c r="I114" s="4">
+      <c r="I114" s="3">
         <v>3.1475921950844588E-2</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B115" s="3"/>
+      <c r="B115" s="7"/>
       <c r="C115" t="s">
         <v>8</v>
       </c>
@@ -3000,18 +2998,18 @@
       <c r="F115">
         <v>103</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="3">
         <v>0.81769911504424775</v>
       </c>
-      <c r="H115" s="4">
+      <c r="H115" s="3">
         <v>7.1513967536618095E-2</v>
       </c>
-      <c r="I115" s="4">
+      <c r="I115" s="3">
         <v>8.8816694329918788E-2</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B116" s="3"/>
+      <c r="B116" s="7"/>
       <c r="C116" t="s">
         <v>9</v>
       </c>
@@ -3021,18 +3019,18 @@
       <c r="F116">
         <v>32</v>
       </c>
-      <c r="G116" s="4">
+      <c r="G116" s="3">
         <v>0.87924528301886795</v>
       </c>
-      <c r="H116" s="4">
+      <c r="H116" s="3">
         <v>0.1330601355112383</v>
       </c>
-      <c r="I116" s="4">
+      <c r="I116" s="3">
         <v>0.15036286230453899</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B117" s="3"/>
+      <c r="B117" s="7"/>
       <c r="C117" t="s">
         <v>10</v>
       </c>
@@ -3042,18 +3040,18 @@
       <c r="F117">
         <v>258</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G117" s="3">
         <v>0.76</v>
       </c>
-      <c r="H117" s="4">
+      <c r="H117" s="3">
         <v>1.3814852492370355E-2</v>
       </c>
-      <c r="I117" s="4">
+      <c r="I117" s="3">
         <v>3.1117579285671049E-2</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C118" t="s">
@@ -3065,18 +3063,18 @@
       <c r="F118">
         <v>29</v>
       </c>
-      <c r="G118" s="4">
+      <c r="G118" s="3">
         <v>0.87168141592920356</v>
       </c>
-      <c r="H118" s="4">
+      <c r="H118" s="3">
         <v>0.1344396176302971</v>
       </c>
-      <c r="I118" s="4">
+      <c r="I118" s="3">
         <v>0.1427989952148746</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B119" s="3"/>
+      <c r="B119" s="7"/>
       <c r="C119" t="s">
         <v>1</v>
       </c>
@@ -3086,18 +3084,18 @@
       <c r="F119">
         <v>134</v>
       </c>
-      <c r="G119" s="4">
+      <c r="G119" s="3">
         <v>0.78996865203761757</v>
       </c>
-      <c r="H119" s="4">
+      <c r="H119" s="3">
         <v>5.272685373871111E-2</v>
       </c>
-      <c r="I119" s="4">
+      <c r="I119" s="3">
         <v>6.1086231323288609E-2</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B120" s="3"/>
+      <c r="B120" s="7"/>
       <c r="C120" t="s">
         <v>2</v>
       </c>
@@ -3107,18 +3105,18 @@
       <c r="F120">
         <v>263</v>
       </c>
-      <c r="G120" s="4">
+      <c r="G120" s="3">
         <v>0.75489282385834111</v>
       </c>
-      <c r="H120" s="4">
+      <c r="H120" s="3">
         <v>1.7651025559434652E-2</v>
       </c>
-      <c r="I120" s="4">
+      <c r="I120" s="3">
         <v>2.6010403144012151E-2</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B121" s="3"/>
+      <c r="B121" s="7"/>
       <c r="C121" t="s">
         <v>3</v>
       </c>
@@ -3128,18 +3126,18 @@
       <c r="F121">
         <v>323</v>
       </c>
-      <c r="G121" s="4">
+      <c r="G121" s="3">
         <v>0.715669014084507</v>
       </c>
-      <c r="H121" s="4">
+      <c r="H121" s="3">
         <v>-2.1572784214399454E-2</v>
       </c>
-      <c r="I121" s="4">
+      <c r="I121" s="3">
         <v>-1.3213406629821955E-2</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B122" s="3"/>
+      <c r="B122" s="7"/>
       <c r="C122" t="s">
         <v>4</v>
       </c>
@@ -3149,18 +3147,18 @@
       <c r="F122">
         <v>371</v>
       </c>
-      <c r="G122" s="4">
+      <c r="G122" s="3">
         <v>0.69211618257261409</v>
       </c>
-      <c r="H122" s="4">
+      <c r="H122" s="3">
         <v>-4.5125615726292367E-2</v>
       </c>
-      <c r="I122" s="4">
+      <c r="I122" s="3">
         <v>-3.6766238141714869E-2</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B123" s="3"/>
+      <c r="B123" s="7"/>
       <c r="C123" t="s">
         <v>5</v>
       </c>
@@ -3170,18 +3168,18 @@
       <c r="F123">
         <v>186</v>
       </c>
-      <c r="G123" s="4">
+      <c r="G123" s="3">
         <v>0.76275510204081631</v>
       </c>
-      <c r="H123" s="4">
+      <c r="H123" s="3">
         <v>2.5513303741909854E-2</v>
       </c>
-      <c r="I123" s="4">
+      <c r="I123" s="3">
         <v>3.3872681326487353E-2</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B124" s="3"/>
+      <c r="B124" s="7"/>
       <c r="C124" t="s">
         <v>6</v>
       </c>
@@ -3191,18 +3189,18 @@
       <c r="F124">
         <v>424</v>
       </c>
-      <c r="G124" s="4">
+      <c r="G124" s="3">
         <v>0.72141918528252302</v>
       </c>
-      <c r="H124" s="4">
+      <c r="H124" s="3">
         <v>-1.5822613016383436E-2</v>
       </c>
-      <c r="I124" s="4">
+      <c r="I124" s="3">
         <v>-7.4632354318059368E-3</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C125" t="s">
@@ -3214,18 +3212,18 @@
       <c r="F125">
         <v>15</v>
       </c>
-      <c r="G125" s="4">
+      <c r="G125" s="3">
         <v>0.74576271186440679</v>
       </c>
-      <c r="H125" s="4">
+      <c r="H125" s="3">
         <v>3.1980133794437315E-2</v>
       </c>
-      <c r="I125" s="4">
+      <c r="I125" s="3">
         <v>1.6880291150077831E-2</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B126" s="3"/>
+      <c r="B126" s="7"/>
       <c r="C126" t="s">
         <v>1</v>
       </c>
@@ -3235,18 +3233,18 @@
       <c r="F126">
         <v>340</v>
       </c>
-      <c r="G126" s="4">
+      <c r="G126" s="3">
         <v>0.7068965517241379</v>
       </c>
-      <c r="H126" s="4">
+      <c r="H126" s="3">
         <v>-6.8860263458315751E-3</v>
       </c>
-      <c r="I126" s="4">
+      <c r="I126" s="3">
         <v>-2.198586899019106E-2</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B127" s="3"/>
+      <c r="B127" s="7"/>
       <c r="C127" t="s">
         <v>2</v>
       </c>
@@ -3256,18 +3254,18 @@
       <c r="F127">
         <v>160</v>
       </c>
-      <c r="G127" s="4">
+      <c r="G127" s="3">
         <v>0.6992481203007519</v>
       </c>
-      <c r="H127" s="4">
+      <c r="H127" s="3">
         <v>-1.4534457769217579E-2</v>
       </c>
-      <c r="I127" s="4">
+      <c r="I127" s="3">
         <v>-2.9634300413577064E-2</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B128" s="3"/>
+      <c r="B128" s="7"/>
       <c r="C128" t="s">
         <v>3</v>
       </c>
@@ -3277,18 +3275,18 @@
       <c r="F128">
         <v>171</v>
       </c>
-      <c r="G128" s="4">
+      <c r="G128" s="3">
         <v>0.76607387140902872</v>
       </c>
-      <c r="H128" s="4">
+      <c r="H128" s="3">
         <v>5.2291293339059242E-2</v>
       </c>
-      <c r="I128" s="4">
+      <c r="I128" s="3">
         <v>3.7191450694699757E-2</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B129" s="3"/>
+      <c r="B129" s="7"/>
       <c r="C129" t="s">
         <v>4</v>
       </c>
@@ -3298,18 +3296,18 @@
       <c r="F129">
         <v>271</v>
       </c>
-      <c r="G129" s="4">
+      <c r="G129" s="3">
         <v>0.70350109409190376</v>
       </c>
-      <c r="H129" s="4">
+      <c r="H129" s="3">
         <v>-1.028148397806572E-2</v>
       </c>
-      <c r="I129" s="4">
+      <c r="I129" s="3">
         <v>-2.5381326622425204E-2</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B130" s="3"/>
+      <c r="B130" s="7"/>
       <c r="C130" t="s">
         <v>5</v>
       </c>
@@ -3319,18 +3317,18 @@
       <c r="F130">
         <v>262</v>
       </c>
-      <c r="G130" s="4">
+      <c r="G130" s="3">
         <v>0.69640787949015059</v>
       </c>
-      <c r="H130" s="4">
+      <c r="H130" s="3">
         <v>-1.7374698579818881E-2</v>
       </c>
-      <c r="I130" s="4">
+      <c r="I130" s="3">
         <v>-3.2474541224178366E-2</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B131" s="3" t="s">
+      <c r="B131" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C131" t="s">
@@ -3342,18 +3340,18 @@
       <c r="F131">
         <v>12</v>
       </c>
-      <c r="G131" s="4">
+      <c r="G131" s="3">
         <v>0.5</v>
       </c>
-      <c r="H131" s="4">
+      <c r="H131" s="3">
         <v>-0.23001310615989512</v>
       </c>
-      <c r="I131" s="4">
+      <c r="I131" s="3">
         <v>-0.22888242071432896</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B132" s="3"/>
+      <c r="B132" s="7"/>
       <c r="C132" t="s">
         <v>1</v>
       </c>
@@ -3363,18 +3361,18 @@
       <c r="F132">
         <v>350</v>
       </c>
-      <c r="G132" s="4">
+      <c r="G132" s="3">
         <v>0.70809007506255217</v>
       </c>
-      <c r="H132" s="4">
+      <c r="H132" s="3">
         <v>-2.1923031097342949E-2</v>
       </c>
-      <c r="I132" s="4">
+      <c r="I132" s="3">
         <v>-2.0792345651776789E-2</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B133" s="3"/>
+      <c r="B133" s="7"/>
       <c r="C133" t="s">
         <v>2</v>
       </c>
@@ -3384,18 +3382,18 @@
       <c r="F133">
         <v>221</v>
       </c>
-      <c r="G133" s="4">
+      <c r="G133" s="3">
         <v>0.74421296296296291</v>
       </c>
-      <c r="H133" s="4">
+      <c r="H133" s="3">
         <v>1.419985680306779E-2</v>
       </c>
-      <c r="I133" s="4">
+      <c r="I133" s="3">
         <v>1.5330542248633949E-2</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B134" s="3"/>
+      <c r="B134" s="7"/>
       <c r="C134" t="s">
         <v>3</v>
       </c>
@@ -3405,18 +3403,18 @@
       <c r="F134">
         <v>241</v>
       </c>
-      <c r="G134" s="4">
+      <c r="G134" s="3">
         <v>0.75025906735751291</v>
       </c>
-      <c r="H134" s="4">
+      <c r="H134" s="3">
         <v>2.024596119761779E-2</v>
       </c>
-      <c r="I134" s="4">
+      <c r="I134" s="3">
         <v>2.137664664318395E-2</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B135" s="3" t="s">
+      <c r="B135" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C135" t="s">
@@ -3428,18 +3426,18 @@
       <c r="F135">
         <v>19</v>
       </c>
-      <c r="G135" s="4">
+      <c r="G135" s="3">
         <v>0.8527131782945736</v>
       </c>
-      <c r="H135" s="4">
+      <c r="H135" s="3">
         <v>9.5925847977831546E-2</v>
       </c>
-      <c r="I135" s="4">
+      <c r="I135" s="3">
         <v>0.12383075758024464</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B136" s="3"/>
+      <c r="B136" s="7"/>
       <c r="C136" t="s">
         <v>1</v>
       </c>
@@ -3449,18 +3447,18 @@
       <c r="F136">
         <v>315</v>
       </c>
-      <c r="G136" s="4">
+      <c r="G136" s="3">
         <v>0.70028544243577551</v>
       </c>
-      <c r="H136" s="4">
+      <c r="H136" s="3">
         <v>-5.650188788096655E-2</v>
       </c>
-      <c r="I136" s="4">
+      <c r="I136" s="3">
         <v>-2.8596978278553453E-2</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B137" s="3"/>
+      <c r="B137" s="7"/>
       <c r="C137" t="s">
         <v>2</v>
       </c>
@@ -3470,18 +3468,18 @@
       <c r="F137">
         <v>147</v>
       </c>
-      <c r="G137" s="4">
+      <c r="G137" s="3">
         <v>0.75335570469798663</v>
       </c>
-      <c r="H137" s="4">
+      <c r="H137" s="3">
         <v>-3.4316256187554295E-3</v>
       </c>
-      <c r="I137" s="4">
+      <c r="I137" s="3">
         <v>2.4473283983657668E-2</v>
       </c>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B138" s="3"/>
+      <c r="B138" s="7"/>
       <c r="C138" t="s">
         <v>3</v>
       </c>
@@ -3491,18 +3489,18 @@
       <c r="F138">
         <v>123</v>
       </c>
-      <c r="G138" s="4">
+      <c r="G138" s="3">
         <v>0.79081632653061229</v>
       </c>
-      <c r="H138" s="4">
+      <c r="H138" s="3">
         <v>3.4028996213870233E-2</v>
       </c>
-      <c r="I138" s="4">
+      <c r="I138" s="3">
         <v>6.193390581628333E-2</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B139" s="3"/>
+      <c r="B139" s="7"/>
       <c r="C139" t="s">
         <v>4</v>
       </c>
@@ -3512,18 +3510,18 @@
       <c r="F139">
         <v>41</v>
       </c>
-      <c r="G139" s="4">
+      <c r="G139" s="3">
         <v>0.85763888888888884</v>
       </c>
-      <c r="H139" s="4">
+      <c r="H139" s="3">
         <v>0.10085155857214678</v>
       </c>
-      <c r="I139" s="4">
+      <c r="I139" s="3">
         <v>0.12875646817455988</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B140" s="3" t="s">
+      <c r="B140" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C140" t="s">
@@ -3535,18 +3533,18 @@
       <c r="F140">
         <v>18</v>
       </c>
-      <c r="G140" s="4">
+      <c r="G140" s="3">
         <v>0.83636363636363631</v>
       </c>
-      <c r="H140" s="4">
+      <c r="H140" s="3">
         <v>8.6248658592672056E-2</v>
       </c>
-      <c r="I140" s="4">
+      <c r="I140" s="3">
         <v>0.10748121564930735</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B141" s="3"/>
+      <c r="B141" s="7"/>
       <c r="C141" t="s">
         <v>1</v>
       </c>
@@ -3556,18 +3554,18 @@
       <c r="F141">
         <v>271</v>
       </c>
-      <c r="G141" s="4">
+      <c r="G141" s="3">
         <v>0.7629046369203849</v>
       </c>
-      <c r="H141" s="4">
+      <c r="H141" s="3">
         <v>1.2789659149420651E-2</v>
       </c>
-      <c r="I141" s="4">
+      <c r="I141" s="3">
         <v>3.4022216206055944E-2</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B142" s="3"/>
+      <c r="B142" s="7"/>
       <c r="C142" t="s">
         <v>2</v>
       </c>
@@ -3577,18 +3575,18 @@
       <c r="F142">
         <v>126</v>
       </c>
-      <c r="G142" s="4">
+      <c r="G142" s="3">
         <v>0.74285714285714288</v>
       </c>
-      <c r="H142" s="4">
+      <c r="H142" s="3">
         <v>-7.2578349138213705E-3</v>
       </c>
-      <c r="I142" s="4">
+      <c r="I142" s="3">
         <v>1.3974722142813922E-2</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B143" s="3"/>
+      <c r="B143" s="7"/>
       <c r="C143" t="s">
         <v>3</v>
       </c>
@@ -3598,18 +3596,18 @@
       <c r="F143">
         <v>118</v>
       </c>
-      <c r="G143" s="4">
+      <c r="G143" s="3">
         <v>0.74065934065934069</v>
       </c>
-      <c r="H143" s="4">
+      <c r="H143" s="3">
         <v>-9.4556371116235605E-3</v>
       </c>
-      <c r="I143" s="4">
+      <c r="I143" s="3">
         <v>1.1776919945011732E-2</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B144" s="3"/>
+      <c r="B144" s="7"/>
       <c r="C144" t="s">
         <v>4</v>
       </c>
@@ -3619,18 +3617,18 @@
       <c r="F144">
         <v>212</v>
       </c>
-      <c r="G144" s="4">
+      <c r="G144" s="3">
         <v>0.7313054499366286</v>
       </c>
-      <c r="H144" s="4">
+      <c r="H144" s="3">
         <v>-1.8809527834335649E-2</v>
       </c>
-      <c r="I144" s="4">
+      <c r="I144" s="3">
         <v>2.4230292222996441E-3</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B145" s="3"/>
+      <c r="B145" s="7"/>
       <c r="C145" t="s">
         <v>5</v>
       </c>
@@ -3640,18 +3638,18 @@
       <c r="F145">
         <v>236</v>
       </c>
-      <c r="G145" s="4">
+      <c r="G145" s="3">
         <v>0.75157894736842101</v>
       </c>
-      <c r="H145" s="4">
+      <c r="H145" s="3">
         <v>1.4639695974567601E-3</v>
       </c>
-      <c r="I145" s="4">
+      <c r="I145" s="3">
         <v>2.2696526654092053E-2</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B146" s="3"/>
+      <c r="B146" s="7"/>
       <c r="C146" t="s">
         <v>6</v>
       </c>
@@ -3661,18 +3659,18 @@
       <c r="F146">
         <v>233</v>
       </c>
-      <c r="G146" s="4">
+      <c r="G146" s="3">
         <v>0.74168514412416853</v>
       </c>
-      <c r="H146" s="4">
+      <c r="H146" s="3">
         <v>-8.4298336467957258E-3</v>
       </c>
-      <c r="I146" s="4">
+      <c r="I146" s="3">
         <v>1.2802723409839567E-2</v>
       </c>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B147" s="3"/>
+      <c r="B147" s="7"/>
       <c r="C147" t="s">
         <v>8</v>
       </c>
@@ -3682,18 +3680,18 @@
       <c r="F147">
         <v>253</v>
       </c>
-      <c r="G147" s="4">
+      <c r="G147" s="3">
         <v>0.73368421052631583</v>
       </c>
-      <c r="H147" s="4">
+      <c r="H147" s="3">
         <v>-1.6430767244648425E-2</v>
       </c>
-      <c r="I147" s="4">
+      <c r="I147" s="3">
         <v>4.8017898119868674E-3</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B148" s="3"/>
+      <c r="B148" s="7"/>
       <c r="C148" t="s">
         <v>9</v>
       </c>
@@ -3703,18 +3701,18 @@
       <c r="F148">
         <v>163</v>
       </c>
-      <c r="G148" s="4">
+      <c r="G148" s="3">
         <v>0.77792915531335149</v>
       </c>
-      <c r="H148" s="4">
+      <c r="H148" s="3">
         <v>2.7814177542387242E-2</v>
       </c>
-      <c r="I148" s="4">
+      <c r="I148" s="3">
         <v>4.9046734599022535E-2</v>
       </c>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C149" t="s">
@@ -3726,18 +3724,18 @@
       <c r="F149">
         <v>2</v>
       </c>
-      <c r="G149" s="4">
+      <c r="G149" s="3">
         <v>0.8571428571428571</v>
       </c>
-      <c r="H149" s="4">
+      <c r="H149" s="3">
         <v>8.8228101922042335E-2</v>
       </c>
-      <c r="I149" s="4">
+      <c r="I149" s="3">
         <v>0.12826043642852814</v>
       </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B150" s="3"/>
+      <c r="B150" s="7"/>
       <c r="C150" t="s">
         <v>1</v>
       </c>
@@ -3747,18 +3745,18 @@
       <c r="F150">
         <v>219</v>
       </c>
-      <c r="G150" s="4">
+      <c r="G150" s="3">
         <v>0.73422330097087374</v>
       </c>
-      <c r="H150" s="4">
+      <c r="H150" s="3">
         <v>-3.4691454249941023E-2</v>
       </c>
-      <c r="I150" s="4">
+      <c r="I150" s="3">
         <v>5.3408802565447777E-3</v>
       </c>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B151" s="3"/>
+      <c r="B151" s="7"/>
       <c r="C151" t="s">
         <v>2</v>
       </c>
@@ -3768,18 +3766,18 @@
       <c r="F151">
         <v>47</v>
       </c>
-      <c r="G151" s="4">
+      <c r="G151" s="3">
         <v>0.80252100840336138</v>
       </c>
-      <c r="H151" s="4">
+      <c r="H151" s="3">
         <v>3.3606253182546619E-2</v>
       </c>
-      <c r="I151" s="4">
+      <c r="I151" s="3">
         <v>7.363858768903242E-2</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B152" s="3"/>
+      <c r="B152" s="7"/>
       <c r="C152" t="s">
         <v>3</v>
       </c>
@@ -3789,18 +3787,18 @@
       <c r="F152">
         <v>110</v>
       </c>
-      <c r="G152" s="4">
+      <c r="G152" s="3">
         <v>0.77505112474437632</v>
       </c>
-      <c r="H152" s="4">
+      <c r="H152" s="3">
         <v>6.1363695235615578E-3</v>
       </c>
-      <c r="I152" s="4">
+      <c r="I152" s="3">
         <v>4.6168704030047358E-2</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B153" s="3"/>
+      <c r="B153" s="7"/>
       <c r="C153" t="s">
         <v>4</v>
       </c>
@@ -3810,18 +3808,18 @@
       <c r="F153">
         <v>160</v>
       </c>
-      <c r="G153" s="4">
+      <c r="G153" s="3">
         <v>0.76811594202898548</v>
       </c>
-      <c r="H153" s="4">
+      <c r="H153" s="3">
         <v>-7.9881319182928401E-4</v>
       </c>
-      <c r="I153" s="4">
+      <c r="I153" s="3">
         <v>3.9233521314656516E-2</v>
       </c>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B154" s="3"/>
+      <c r="B154" s="7"/>
       <c r="C154" t="s">
         <v>5</v>
       </c>
@@ -3831,18 +3829,32 @@
       <c r="F154">
         <v>137</v>
       </c>
-      <c r="G154" s="4">
+      <c r="G154" s="3">
         <v>0.79429429429429432</v>
       </c>
-      <c r="H154" s="4">
+      <c r="H154" s="3">
         <v>2.5379539073479562E-2</v>
       </c>
-      <c r="I154" s="4">
+      <c r="I154" s="3">
         <v>6.5411873579965363E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B101:B107"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="B53:B61"/>
+    <mergeCell ref="B62:B69"/>
+    <mergeCell ref="B70:B77"/>
+    <mergeCell ref="B78:B85"/>
+    <mergeCell ref="B86:B93"/>
+    <mergeCell ref="B94:B100"/>
     <mergeCell ref="B140:B148"/>
     <mergeCell ref="B149:B154"/>
     <mergeCell ref="B108:B117"/>
@@ -3850,20 +3862,6 @@
     <mergeCell ref="B125:B130"/>
     <mergeCell ref="B131:B134"/>
     <mergeCell ref="B135:B139"/>
-    <mergeCell ref="B62:B69"/>
-    <mergeCell ref="B70:B77"/>
-    <mergeCell ref="B78:B85"/>
-    <mergeCell ref="B86:B93"/>
-    <mergeCell ref="B94:B100"/>
-    <mergeCell ref="B101:B107"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B53:B61"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>